<commit_message>
Fix dates bug and country codes bug
Montenegro, RDC y Rumania no aparecian
los cortesd de fechas no estaban bien
</commit_message>
<xml_diff>
--- a/Data/Data_Raw/Country codes & metadata/wbcodes1.xlsx
+++ b/Data/Data_Raw/Country codes & metadata/wbcodes1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llohi\Documents\WB\Data Portal\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laboral\World Bank\Data-Portal-Brief-Generator\Data\Data_Raw\Country codes &amp; metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C697EE-5C85-43DE-8BFB-2188B6B2C054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADA7720-9344-48D8-9B21-FB06C48F257D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{70D08953-D62D-4E72-858A-F8E9F049F74C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{70D08953-D62D-4E72-858A-F8E9F049F74C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -338,9 +338,6 @@
     <t>Comoros</t>
   </si>
   <si>
-    <t>ZAR</t>
-  </si>
-  <si>
     <t>Congo, Dem. Rep.</t>
   </si>
   <si>
@@ -986,9 +983,6 @@
     <t>Mongolia</t>
   </si>
   <si>
-    <t>MNT</t>
-  </si>
-  <si>
     <t>Montenegro</t>
   </si>
   <si>
@@ -1202,9 +1196,6 @@
     <t>Reunion</t>
   </si>
   <si>
-    <t>ROM</t>
-  </si>
-  <si>
     <t>Romania</t>
   </si>
   <si>
@@ -1668,6 +1659,15 @@
   </si>
   <si>
     <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>ROU</t>
+  </si>
+  <si>
+    <t>COD</t>
+  </si>
+  <si>
+    <t>MNE</t>
   </si>
 </sst>
 </file>
@@ -1745,7 +1745,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2043,13 +2043,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E4BC82-C844-466D-B224-73F53A851211}">
   <dimension ref="A1:B272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="H201" sqref="H201"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="A160" sqref="A160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="27" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="27" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="27" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="27" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="54" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="27" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="51" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="54" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="27" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>70</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>76</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>78</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="27" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>80</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="27" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>90</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="27" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>92</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>96</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>98</v>
       </c>
@@ -2449,1780 +2449,1780 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="27" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="3" t="s">
+    </row>
+    <row r="52" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="B52" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="3" t="s">
+    </row>
+    <row r="53" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="B53" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="3" t="s">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="B54" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B54" s="3" t="s">
+    </row>
+    <row r="55" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="B55" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="3" t="s">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="B56" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="3" t="s">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="B57" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B57" s="3" t="s">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="B58" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B58" s="3" t="s">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="B59" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B59" s="3" t="s">
+    </row>
+    <row r="60" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="B60" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B60" s="3" t="s">
+    </row>
+    <row r="61" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="B61" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B61" s="3" t="s">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="B62" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B62" s="3" t="s">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="B63" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B63" s="3" t="s">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="B64" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B64" s="3" t="s">
+    </row>
+    <row r="65" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="B65" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B65" s="3" t="s">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="B66" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B66" s="3" t="s">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+      <c r="B67" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B67" s="3" t="s">
+    </row>
+    <row r="68" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+      <c r="B68" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B68" s="3" t="s">
+    </row>
+    <row r="69" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="B69" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B69" s="3" t="s">
+    </row>
+    <row r="70" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="B70" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B70" s="3" t="s">
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="B71" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B71" s="3" t="s">
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+      <c r="B72" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B72" s="3" t="s">
+    </row>
+    <row r="73" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+      <c r="B73" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B73" s="3" t="s">
+    </row>
+    <row r="74" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="B74" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B74" s="3" t="s">
+    </row>
+    <row r="75" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="B75" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B75" s="3" t="s">
+    </row>
+    <row r="76" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+      <c r="B76" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B76" s="3" t="s">
+    </row>
+    <row r="77" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+      <c r="B77" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B77" s="3" t="s">
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+      <c r="B78" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B78" s="3" t="s">
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+      <c r="B79" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B79" s="3" t="s">
+    </row>
+    <row r="80" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+      <c r="B80" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B80" s="3" t="s">
+    </row>
+    <row r="81" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+      <c r="B81" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B81" s="3" t="s">
+    </row>
+    <row r="82" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+      <c r="B82" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B82" s="3" t="s">
+    </row>
+    <row r="83" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="B83" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B83" s="3" t="s">
+    </row>
+    <row r="84" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+      <c r="B84" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B84" s="3" t="s">
+    </row>
+    <row r="85" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+      <c r="B85" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B85" s="3" t="s">
+    </row>
+    <row r="86" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+      <c r="B86" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B86" s="3" t="s">
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+      <c r="B87" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="B87" s="3" t="s">
+    </row>
+    <row r="88" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+      <c r="B88" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B88" s="3" t="s">
+    </row>
+    <row r="89" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+      <c r="B89" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B89" s="3" t="s">
+    </row>
+    <row r="90" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+      <c r="B90" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B90" s="3" t="s">
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+      <c r="B91" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B91" s="3" t="s">
+    </row>
+    <row r="92" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+      <c r="B92" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B92" s="3" t="s">
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+      <c r="B93" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B93" s="3" t="s">
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+      <c r="B94" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="B94" s="3" t="s">
+    </row>
+    <row r="95" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+      <c r="B95" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B95" s="3" t="s">
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+      <c r="B96" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B96" s="3" t="s">
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+      <c r="B97" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="B97" s="3" t="s">
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+      <c r="B98" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B98" s="3" t="s">
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+      <c r="B99" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B99" s="3" t="s">
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+      <c r="B100" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="B100" s="3" t="s">
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="B101" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B101" s="3" t="s">
+    </row>
+    <row r="102" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A102" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+      <c r="B102" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B102" s="3" t="s">
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+      <c r="B103" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="B103" s="3" t="s">
+    </row>
+    <row r="104" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A104" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+      <c r="B104" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="B104" s="3" t="s">
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+      <c r="B105" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B105" s="3" t="s">
+    </row>
+    <row r="106" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A106" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+      <c r="B106" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B106" s="3" t="s">
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" s="1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+      <c r="B107" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B107" s="3" t="s">
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" s="1" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+      <c r="B108" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="B108" s="3" t="s">
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" s="1" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+      <c r="B109" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B109" s="3" t="s">
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+      <c r="B110" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="B110" s="3" t="s">
+    </row>
+    <row r="111" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A111" s="1" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+      <c r="B111" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B111" s="3" t="s">
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+      <c r="B112" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="B112" s="3" t="s">
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" s="1" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+      <c r="B113" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B113" s="3" t="s">
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" s="1" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+      <c r="B114" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="B114" s="3" t="s">
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
+      <c r="B115" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B115" s="3" t="s">
+    </row>
+    <row r="116" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A116" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+      <c r="B116" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="B116" s="3" t="s">
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
+      <c r="B117" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="B117" s="3" t="s">
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+      <c r="B118" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="B118" s="3" t="s">
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" s="1" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+      <c r="B119" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="B119" s="3" t="s">
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+      <c r="B120" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="B120" s="3" t="s">
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" s="1" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+      <c r="B121" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="B121" s="3" t="s">
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" s="1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
+      <c r="B122" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="B122" s="3" t="s">
+    </row>
+    <row r="123" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A123" s="1" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
+      <c r="B123" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B123" s="3" t="s">
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" s="1" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
+      <c r="B124" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="B124" s="3" t="s">
+    </row>
+    <row r="125" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A125" s="1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
+      <c r="B125" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="B125" s="3" t="s">
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" s="1" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
+      <c r="B126" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B126" s="3" t="s">
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
+      <c r="B127" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B127" s="3" t="s">
+    </row>
+    <row r="128" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A128" s="1" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
+      <c r="B128" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B128" s="3" t="s">
+    </row>
+    <row r="129" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A129" s="1" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
+      <c r="B129" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B129" s="3" t="s">
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
+      <c r="B130" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B130" s="3" t="s">
+    </row>
+    <row r="131" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A131" s="1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
+      <c r="B131" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="B131" s="3" t="s">
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" s="1" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
+      <c r="B132" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B132" s="3" t="s">
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" s="1" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
+      <c r="B133" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B133" s="3" t="s">
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" s="1" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
+      <c r="B134" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="B134" s="3" t="s">
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" s="1" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
+      <c r="B135" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="B135" s="3" t="s">
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
+      <c r="B136" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="B136" s="3" t="s">
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
+      <c r="B137" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B137" s="3" t="s">
+    </row>
+    <row r="138" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A138" s="1" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
+      <c r="B138" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="B138" s="3" t="s">
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" s="1" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
+      <c r="B139" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="B139" s="3" t="s">
+    </row>
+    <row r="140" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A140" s="1" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A140" s="1" t="s">
+      <c r="B140" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="B140" s="3" t="s">
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="1" t="s">
+      <c r="B141" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="B141" s="3" t="s">
+    </row>
+    <row r="142" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A142" s="1" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
+      <c r="B142" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="B142" s="3" t="s">
+    </row>
+    <row r="143" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A143" s="1" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A143" s="1" t="s">
+      <c r="B143" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B143" s="3" t="s">
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" s="1" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="1" t="s">
+      <c r="B144" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="B144" s="3" t="s">
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" s="1" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
+      <c r="B145" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="B145" s="3" t="s">
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A146" s="1" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
+      <c r="B146" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="B146" s="3" t="s">
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147" s="1" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="1" t="s">
+      <c r="B147" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="B147" s="3" t="s">
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A148" s="1" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="s">
+      <c r="B148" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="B148" s="3" t="s">
+    </row>
+    <row r="149" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A149" s="1" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
+      <c r="B149" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="B149" s="3" t="s">
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A150" s="1" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
+      <c r="B150" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="B150" s="3" t="s">
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A151" s="1" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="1" t="s">
+      <c r="B151" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="B151" s="3" t="s">
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A152" s="1" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="1" t="s">
+      <c r="B152" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="B152" s="3" t="s">
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A153" s="1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="1" t="s">
+      <c r="B153" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="B153" s="3" t="s">
+    </row>
+    <row r="154" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A154" s="1" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="s">
+      <c r="B154" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="B154" s="3" t="s">
+    </row>
+    <row r="155" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A155" s="1" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A155" s="1" t="s">
+      <c r="B155" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="B155" s="3" t="s">
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A156" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="1" t="s">
+      <c r="B156" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="B156" s="3" t="s">
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A157" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="1" t="s">
+      <c r="B157" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="B157" s="3" t="s">
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A158" s="1" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
+      <c r="B158" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="B158" s="3" t="s">
+    </row>
+    <row r="159" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A159" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B159" s="3" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A159" s="1" t="s">
+    <row r="160" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A160" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="B159" s="3" t="s">
+      <c r="B160" s="3" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="1" t="s">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A161" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="B160" s="3" t="s">
+      <c r="B161" s="3" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="1" t="s">
+    <row r="162" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A162" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="B161" s="3" t="s">
+      <c r="B162" s="3" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A163" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B162" s="3" t="s">
+      <c r="B163" s="3" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="1" t="s">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A164" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="B163" s="3" t="s">
+      <c r="B164" s="3" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="1" t="s">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A165" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="B164" s="3" t="s">
+      <c r="B165" s="3" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="1" t="s">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A166" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="B165" s="3" t="s">
+      <c r="B166" s="3" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="1" t="s">
+    <row r="167" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A167" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B166" s="3" t="s">
+      <c r="B167" s="3" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A167" s="1" t="s">
+    <row r="168" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A168" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="B167" s="3" t="s">
+      <c r="B168" s="3" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A168" s="1" t="s">
+    <row r="169" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A169" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B168" s="3" t="s">
+      <c r="B169" s="3" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A169" s="1" t="s">
+    <row r="170" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A170" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="B169" s="3" t="s">
+      <c r="B170" s="3" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A170" s="1" t="s">
+    <row r="171" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A171" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="B170" s="3" t="s">
+      <c r="B171" s="3" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A171" s="1" t="s">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A172" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="B171" s="3" t="s">
+      <c r="B172" s="3" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" s="1" t="s">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A173" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B172" s="3" t="s">
+      <c r="B173" s="3" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="1" t="s">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A174" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="B173" s="3" t="s">
+      <c r="B174" s="3" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" s="1" t="s">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A175" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B174" s="3" t="s">
+      <c r="B175" s="3" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="1" t="s">
+    <row r="176" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A176" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="B175" s="3" t="s">
+      <c r="B176" s="3" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A176" s="1" t="s">
+    <row r="177" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A177" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="B176" s="3" t="s">
+      <c r="B177" s="3" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A177" s="1" t="s">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A178" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="B177" s="3" t="s">
+      <c r="B178" s="3" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" s="1" t="s">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A179" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="B178" s="3" t="s">
+      <c r="B179" s="3" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="1" t="s">
+    <row r="180" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A180" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="B179" s="3" t="s">
+      <c r="B180" s="3" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A180" s="1" t="s">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A181" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="B180" s="3" t="s">
+      <c r="B181" s="3" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="1" t="s">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A182" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="B181" s="3" t="s">
+      <c r="B182" s="3" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" s="1" t="s">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A183" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="B182" s="3" t="s">
+      <c r="B183" s="3" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="1" t="s">
+    <row r="184" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A184" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="B183" s="3" t="s">
+      <c r="B184" s="3" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A184" s="1" t="s">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A185" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="B184" s="3" t="s">
+      <c r="B185" s="3" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="1" t="s">
+    <row r="186" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A186" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="B185" s="3" t="s">
+      <c r="B186" s="3" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A186" s="1" t="s">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A187" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="B186" s="3" t="s">
+      <c r="B187" s="3" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="1" t="s">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A188" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="B187" s="3" t="s">
+      <c r="B188" s="3" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A188" s="1" t="s">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A189" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="B188" s="3" t="s">
+      <c r="B189" s="3" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="1" t="s">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A190" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="B189" s="3" t="s">
+      <c r="B190" s="3" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A190" s="1" t="s">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A191" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="B190" s="3" t="s">
+      <c r="B191" s="3" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="1" t="s">
+    <row r="192" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A192" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B191" s="3" t="s">
+      <c r="B192" s="3" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A192" s="1" t="s">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A193" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="B192" s="3" t="s">
+      <c r="B193" s="3" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" s="1" t="s">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A194" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="B193" s="3" t="s">
+      <c r="B194" s="3" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" s="1" t="s">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A195" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="B195" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="B194" s="3" t="s">
+    </row>
+    <row r="196" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A196" s="1" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" s="1" t="s">
+      <c r="B196" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="B195" s="3" t="s">
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A197" s="1" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="196" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A196" s="1" t="s">
+      <c r="B197" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="B196" s="3" t="s">
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A198" s="1" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" s="1" t="s">
+      <c r="B198" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="B197" s="3" t="s">
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A199" s="1" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="1" t="s">
+      <c r="B199" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="B198" s="3" t="s">
+    </row>
+    <row r="200" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A200" s="1" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A199" s="1" t="s">
+      <c r="B200" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="B199" s="3" t="s">
+    </row>
+    <row r="201" spans="1:2" ht="54" x14ac:dyDescent="0.35">
+      <c r="A201" s="1" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="200" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A200" s="1" t="s">
+      <c r="B201" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="B200" s="3" t="s">
+    </row>
+    <row r="202" spans="1:2" ht="54" x14ac:dyDescent="0.35">
+      <c r="A202" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A203" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A204" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A205" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A206" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A207" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A208" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A209" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A210" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A211" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A212" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A213" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A214" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A215" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A216" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A217" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A218" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A219" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B219" s="3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A220" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A221" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B221" s="3" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A222" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B222" s="3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A223" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A224" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A225" s="1" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="201" spans="1:2" ht="51" x14ac:dyDescent="0.25">
-      <c r="A201" s="1" t="s">
+      <c r="B225" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="B201" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" ht="51" x14ac:dyDescent="0.25">
-      <c r="A202" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="B202" s="3" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A203" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="B203" s="3" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="B204" s="3" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A205" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="B205" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A206" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="B206" s="3" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A207" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A208" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="B208" s="3" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="B209" s="3" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="B210" s="3" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="B211" s="3" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A212" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="B212" s="3" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="B213" s="3" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="B214" s="3" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A215" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="B215" s="3" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A216" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="B216" s="3" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A217" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="B217" s="3" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A218" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="B218" s="3" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A219" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="B219" s="3" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A220" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="B220" s="3" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A221" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="B221" s="3" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A222" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="B222" s="3" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A223" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="B223" s="3" t="s">
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A226" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" s="1" t="s">
+      <c r="B226" s="3" t="s">
         <v>448</v>
       </c>
-      <c r="B224" s="3" t="s">
+    </row>
+    <row r="227" spans="1:2" ht="67.5" x14ac:dyDescent="0.35">
+      <c r="A227" s="1" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="225" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A225" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="B225" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A226" s="1" t="s">
+      <c r="B227" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="B226" s="3" t="s">
+    </row>
+    <row r="228" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A228" s="1" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="227" spans="1:2" ht="51" x14ac:dyDescent="0.25">
-      <c r="A227" s="1" t="s">
+      <c r="B228" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="B227" s="3" t="s">
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A229" s="1" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="228" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A228" s="1" t="s">
+      <c r="B229" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="B228" s="3" t="s">
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A230" s="1" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A229" s="1" t="s">
+      <c r="B230" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="B229" s="3" t="s">
+    </row>
+    <row r="231" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A231" s="1" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A230" s="1" t="s">
+      <c r="B231" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="B230" s="3" t="s">
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A232" s="1" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="231" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A231" s="1" t="s">
+      <c r="B232" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="B231" s="3" t="s">
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A233" s="1" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A232" s="1" t="s">
+      <c r="B233" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="B232" s="3" t="s">
+    </row>
+    <row r="234" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A234" s="1" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" s="1" t="s">
+      <c r="B234" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="B233" s="3" t="s">
+    </row>
+    <row r="235" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A235" s="1" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="234" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A234" s="1" t="s">
+      <c r="B235" s="3" t="s">
         <v>466</v>
       </c>
-      <c r="B234" s="3" t="s">
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A236" s="1" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="235" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A235" s="1" t="s">
+      <c r="B236" s="3" t="s">
         <v>468</v>
       </c>
-      <c r="B235" s="3" t="s">
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A237" s="1" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" s="1" t="s">
+      <c r="B237" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="B236" s="3" t="s">
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A238" s="1" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="1" t="s">
+      <c r="B238" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="B237" s="3" t="s">
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A239" s="1" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" s="1" t="s">
+      <c r="B239" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="B238" s="3" t="s">
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A240" s="1" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" s="1" t="s">
+      <c r="B240" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="B239" s="3" t="s">
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A241" s="1" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A240" s="1" t="s">
+      <c r="B241" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="B240" s="4" t="s">
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A242" s="1" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" s="1" t="s">
+      <c r="B242" s="3" t="s">
         <v>480</v>
       </c>
-      <c r="B241" s="3" t="s">
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A243" s="1" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A242" s="1" t="s">
+      <c r="B243" s="3" t="s">
         <v>482</v>
       </c>
-      <c r="B242" s="3" t="s">
+    </row>
+    <row r="244" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A244" s="1" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" s="1" t="s">
+      <c r="B244" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="B243" s="3" t="s">
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A245" s="1" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="244" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A244" s="1" t="s">
+      <c r="B245" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="B244" s="3" t="s">
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A246" s="1" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A245" s="1" t="s">
+      <c r="B246" s="3" t="s">
         <v>488</v>
       </c>
-      <c r="B245" s="3" t="s">
+    </row>
+    <row r="247" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A247" s="1" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" s="1" t="s">
+      <c r="B247" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="B246" s="3" t="s">
+    </row>
+    <row r="248" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A248" s="1" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="247" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A247" s="1" t="s">
+      <c r="B248" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="B247" s="3" t="s">
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A249" s="1" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="248" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A248" s="1" t="s">
+      <c r="B249" s="3" t="s">
         <v>494</v>
       </c>
-      <c r="B248" s="3" t="s">
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A250" s="1" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" s="1" t="s">
+      <c r="B250" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="B249" s="3" t="s">
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A251" s="1" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="1" t="s">
+      <c r="B251" s="3" t="s">
         <v>498</v>
       </c>
-      <c r="B250" s="3" t="s">
+    </row>
+    <row r="252" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A252" s="1" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="1" t="s">
+      <c r="B252" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="B251" s="3" t="s">
+    </row>
+    <row r="253" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A253" s="1" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="252" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A252" s="1" t="s">
+      <c r="B253" s="3" t="s">
         <v>502</v>
       </c>
-      <c r="B252" s="3" t="s">
+    </row>
+    <row r="254" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A254" s="1" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="253" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A253" s="1" t="s">
+      <c r="B254" s="3" t="s">
         <v>504</v>
       </c>
-      <c r="B253" s="3" t="s">
+    </row>
+    <row r="255" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A255" s="1" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="254" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A254" s="1" t="s">
+      <c r="B255" s="3" t="s">
         <v>506</v>
       </c>
-      <c r="B254" s="3" t="s">
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A256" s="1" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="255" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A255" s="1" t="s">
+      <c r="B256" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="B255" s="3" t="s">
+    </row>
+    <row r="257" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A257" s="1" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" s="1" t="s">
+      <c r="B257" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="B256" s="3" t="s">
+    </row>
+    <row r="258" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A258" s="1" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="257" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A257" s="1" t="s">
+      <c r="B258" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="B257" s="3" t="s">
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A259" s="1" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258" s="1" t="s">
+      <c r="B259" s="3" t="s">
         <v>514</v>
       </c>
-      <c r="B258" s="3" t="s">
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A260" s="1" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" s="1" t="s">
+      <c r="B260" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="B259" s="3" t="s">
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A261" s="1" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A260" s="1" t="s">
+      <c r="B261" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="B260" s="3" t="s">
+    </row>
+    <row r="262" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A262" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A261" s="1" t="s">
+      <c r="B262" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="B261" s="3" t="s">
+    </row>
+    <row r="263" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A263" s="1" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="262" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A262" s="1" t="s">
+      <c r="B263" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="B262" s="3" t="s">
+    </row>
+    <row r="264" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A264" s="1" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="263" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A263" s="1" t="s">
+      <c r="B264" s="3" t="s">
         <v>524</v>
       </c>
-      <c r="B263" s="3" t="s">
+    </row>
+    <row r="265" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A265" s="1" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="264" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A264" s="1" t="s">
+      <c r="B265" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="B264" s="3" t="s">
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A266" s="1" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="265" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A265" s="1" t="s">
+      <c r="B266" s="3" t="s">
         <v>528</v>
       </c>
-      <c r="B265" s="3" t="s">
+    </row>
+    <row r="267" spans="1:2" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A267" s="1" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="1" t="s">
+      <c r="B267" s="3" t="s">
         <v>530</v>
       </c>
-      <c r="B266" s="3" t="s">
+    </row>
+    <row r="268" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A268" s="1" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="267" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A267" s="1" t="s">
+      <c r="B268" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="B267" s="3" t="s">
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A269" s="1" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="268" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A268" s="1" t="s">
+      <c r="B269" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="B268" s="3" t="s">
+    </row>
+    <row r="270" spans="1:2" ht="54" x14ac:dyDescent="0.35">
+      <c r="A270" s="1" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="1" t="s">
+      <c r="B270" s="3" t="s">
         <v>536</v>
       </c>
-      <c r="B269" s="3" t="s">
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A271" s="1" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="270" spans="1:2" ht="51" x14ac:dyDescent="0.25">
-      <c r="A270" s="1" t="s">
+      <c r="B271" s="3" t="s">
         <v>538</v>
       </c>
-      <c r="B270" s="3" t="s">
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A272" s="1" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="1" t="s">
+      <c r="B272" s="3" t="s">
         <v>540</v>
-      </c>
-      <c r="B271" s="3" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="B272" s="3" t="s">
-        <v>543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>